<commit_message>
Added Tests for updates read create
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wessel\Documents\UiPath\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDF74A-FF1A-4C95-A2AF-0A05AA0341A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,13 +283,13 @@
     <t>Create Test Passed</t>
   </si>
   <si>
+    <t>Update Test Passed</t>
+  </si>
+  <si>
+    <t>Delete Test Passed</t>
+  </si>
+  <si>
     <t>Read Test Passed</t>
-  </si>
-  <si>
-    <t>Update Test Passed</t>
-  </si>
-  <si>
-    <t>Delete Test Passed</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,13 +1147,13 @@
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,13 +1314,13 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
         <v>0</v>
@@ -1331,13 +1331,13 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
         <v>0</v>
@@ -1348,13 +1348,13 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
         <v>0</v>
@@ -1365,13 +1365,13 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -1382,13 +1382,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1549,5 +1549,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>